<commit_message>
commiting changes of agent aux report
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/OCMAnalysisCountReportData.xlsx
+++ b/ocms/src/test/resources/TestData/OCMAnalysisCountReportData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D5F3FF-8884-4E25-BA35-9019010577CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7C3BC0-C818-4992-A285-93DA27A81991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Show" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="50">
   <si>
     <t>Report Channel</t>
   </si>
@@ -104,16 +104,61 @@
     <t>OCM Analysis Count Report</t>
   </si>
   <si>
+    <t>17-06-2020 00:00:00</t>
+  </si>
+  <si>
+    <t>18-06-2020 00:00:00</t>
+  </si>
+  <si>
+    <t>17-06-2020 00:00:01</t>
+  </si>
+  <si>
+    <t>17-06-2020 00:00:02</t>
+  </si>
+  <si>
+    <t>17-06-2020 00:00:03</t>
+  </si>
+  <si>
+    <t>17-06-2020 00:00:04</t>
+  </si>
+  <si>
+    <t>18-06-2020 00:00:01</t>
+  </si>
+  <si>
+    <t>18-06-2020 00:00:02</t>
+  </si>
+  <si>
+    <t>18-06-2020 00:00:03</t>
+  </si>
+  <si>
+    <t>18-06-2020 00:00:04</t>
+  </si>
+  <si>
     <t>Menu</t>
   </si>
   <si>
+    <t>5006_2</t>
+  </si>
+  <si>
     <t>HDFC</t>
   </si>
   <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
     <t>Does not contain</t>
+  </si>
+  <si>
+    <t>01-07-2020 00:00:00</t>
+  </si>
+  <si>
+    <t>01-10-2020 00:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">SELECT [MENU] as [Menu],sum([ACCESSCOUNT]) AS [AccessCount] ,sum([INVALIDINPUT]) AS [Invalid Input] ,
@@ -168,28 +213,19 @@
 </t>
   </si>
   <si>
-    <t>16-03-2021 00:00:00</t>
-  </si>
-  <si>
-    <t>17-03-2021 00:00:00</t>
-  </si>
-  <si>
-    <t>01-03-2021 00:00:00</t>
-  </si>
-  <si>
-    <t>01-04-2021 00:00:00</t>
-  </si>
-  <si>
-    <t>UOBMGetIntent</t>
-  </si>
-  <si>
-    <t>MainMenu</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>R</t>
+    <t>Is not equal to</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Starts with</t>
+  </si>
+  <si>
+    <t>Ends with</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -225,7 +261,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -523,7 +561,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -545,10 +583,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -562,10 +600,10 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -580,7 +618,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -588,7 +626,7 @@
     <col min="2" max="2" width="22.26953125" customWidth="1"/>
     <col min="3" max="3" width="16.7265625" customWidth="1"/>
     <col min="4" max="4" width="19.453125" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="17.26953125" customWidth="1"/>
     <col min="8" max="8" width="24.1796875" customWidth="1"/>
@@ -596,205 +634,205 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="F5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="F6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="F7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="G7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -808,7 +846,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -834,17 +872,17 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>30</v>
+      <c r="D2" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -856,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -886,20 +924,20 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>33</v>
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -912,7 +950,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -937,26 +975,22 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="D2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -968,7 +1002,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -996,27 +1030,27 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1027,15 +1061,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
     <col min="3" max="3" width="11.81640625" customWidth="1"/>
     <col min="4" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.453125" customWidth="1"/>
@@ -1047,73 +1081,218 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>27</v>
+      <c r="E3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1125,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1139,43 +1318,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>29</v>
+      <c r="A2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>